<commit_message>
Correction of errors and improvements
</commit_message>
<xml_diff>
--- a/Case_studies/Montefrio/sampling/optimal_sampling_points.xlsx
+++ b/Case_studies/Montefrio/sampling/optimal_sampling_points.xlsx
@@ -447,82 +447,82 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>410107.5</v>
+        <v>410157.5</v>
       </c>
       <c r="B2" t="n">
-        <v>4132482.5</v>
+        <v>4132427.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>410297.5</v>
+        <v>410202.5</v>
       </c>
       <c r="B3" t="n">
-        <v>4132717.5</v>
+        <v>4132477.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>410072.5</v>
+        <v>410412.5</v>
       </c>
       <c r="B4" t="n">
-        <v>4132547.5</v>
+        <v>4132697.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>410277.5</v>
+        <v>409997.5</v>
       </c>
       <c r="B5" t="n">
-        <v>4132627.5</v>
+        <v>4132372.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>410442.5</v>
+        <v>410312.5</v>
       </c>
       <c r="B6" t="n">
-        <v>4132662.5</v>
+        <v>4132707.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>410332.5</v>
+        <v>410112.5</v>
       </c>
       <c r="B7" t="n">
-        <v>4132527.5</v>
+        <v>4132377.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>410087.5</v>
+        <v>410247.5</v>
       </c>
       <c r="B8" t="n">
-        <v>4132447.5</v>
+        <v>4132707.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>410287.5</v>
+        <v>410392.5</v>
       </c>
       <c r="B9" t="n">
-        <v>4132627.5</v>
+        <v>4132632.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>410217.5</v>
+        <v>410082.5</v>
       </c>
       <c r="B10" t="n">
-        <v>4132742.5</v>
+        <v>4132512.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>410257.5</v>
+        <v>409967.5</v>
       </c>
       <c r="B11" t="n">
-        <v>4132487.5</v>
+        <v>4132392.5</v>
       </c>
     </row>
     <row r="12">
@@ -530,159 +530,159 @@
         <v>410272.5</v>
       </c>
       <c r="B12" t="n">
-        <v>4132537.5</v>
+        <v>4132617.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>410187.5</v>
+        <v>410207.5</v>
       </c>
       <c r="B13" t="n">
-        <v>4132547.5</v>
+        <v>4132632.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>409917.5</v>
+        <v>410487.5</v>
       </c>
       <c r="B14" t="n">
-        <v>4132497.5</v>
+        <v>4132637.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>410477.5</v>
+        <v>409977.5</v>
       </c>
       <c r="B15" t="n">
-        <v>4132622.5</v>
+        <v>4132442.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>410147.5</v>
+        <v>410132.5</v>
       </c>
       <c r="B16" t="n">
-        <v>4132582.5</v>
+        <v>4132392.5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>410272.5</v>
+        <v>410292.5</v>
       </c>
       <c r="B17" t="n">
-        <v>4132577.5</v>
+        <v>4132592.5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>410057.5</v>
+        <v>409937.5</v>
       </c>
       <c r="B18" t="n">
-        <v>4132377.5</v>
+        <v>4132492.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>410322.5</v>
+        <v>410127.5</v>
       </c>
       <c r="B19" t="n">
-        <v>4132652.5</v>
+        <v>4132532.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>409842.5</v>
+        <v>410312.5</v>
       </c>
       <c r="B20" t="n">
-        <v>4132417.5</v>
+        <v>4132662.5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>410012.5</v>
+        <v>410122.5</v>
       </c>
       <c r="B21" t="n">
-        <v>4132442.5</v>
+        <v>4132567.5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>410067.5</v>
+        <v>409927.5</v>
       </c>
       <c r="B22" t="n">
-        <v>4132662.5</v>
+        <v>4132442.5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>410082.5</v>
+        <v>409792.5</v>
       </c>
       <c r="B23" t="n">
-        <v>4132497.5</v>
+        <v>4132352.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>410082.5</v>
+        <v>410112.5</v>
       </c>
       <c r="B24" t="n">
-        <v>4132447.5</v>
+        <v>4132782.5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>410027.5</v>
+        <v>409822.5</v>
       </c>
       <c r="B25" t="n">
-        <v>4132662.5</v>
+        <v>4132362.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>410157.5</v>
+        <v>409892.5</v>
       </c>
       <c r="B26" t="n">
-        <v>4132817.5</v>
+        <v>4132467.5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>409897.5</v>
+        <v>409987.5</v>
       </c>
       <c r="B27" t="n">
-        <v>4132437.5</v>
+        <v>4132502.5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>410232.5</v>
+        <v>409972.5</v>
       </c>
       <c r="B28" t="n">
-        <v>4132657.5</v>
+        <v>4132597.5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>410072.5</v>
+        <v>410002.5</v>
       </c>
       <c r="B29" t="n">
-        <v>4132627.5</v>
+        <v>4132592.5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>410137.5</v>
+        <v>409887.5</v>
       </c>
       <c r="B30" t="n">
-        <v>4132612.5</v>
+        <v>4132422.5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>409987.5</v>
+        <v>410087.5</v>
       </c>
       <c r="B31" t="n">
-        <v>4132557.5</v>
+        <v>4132432.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>